<commit_message>
commit all crm gui
</commit_message>
<xml_diff>
--- a/testdata/testscriptdata.xlsx
+++ b/testdata/testscriptdata.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathi\WorkSpace-Tekpyramid\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathi\Eclipse-NewWorkspace\ComcastCRMGUIFRAMEWORK\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B32AC92-D97F-4C76-8D84-90C3F158AB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B95187-C6B2-4DA4-B2F1-6253CC364A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{87CE2105-3880-4D7B-B5B2-F4C38CF5BAFA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{87CE2105-3880-4D7B-B5B2-F4C38CF5BAFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="org" sheetId="2" r:id="rId2"/>
     <sheet name="contact" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="product" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>Brand name</t>
   </si>
@@ -184,6 +185,24 @@
   </si>
   <si>
     <t>Contact  Last Name</t>
+  </si>
+  <si>
+    <t>Product name</t>
+  </si>
+  <si>
+    <t>Apple iPhone 14 Plus (Blue, 128 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 12 (Blue, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 15 (Blue, 128 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 14 Plus (Midnight, 128 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 15 Plus (Pink, 128 GB)</t>
   </si>
 </sst>
 </file>
@@ -866,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EC1516-073E-4E62-AA81-DC51EF5E8CD0}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -929,4 +948,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068080E4-7049-4E7A-8B17-D8376118FA92}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>